<commit_message>
v2 and v3 iterations of the CNN.
At this stage, v3_2 is our best and most promising model. see evaluation images for visual displays
</commit_message>
<xml_diff>
--- a/v1/outputs.xlsx
+++ b/v1/outputs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mattb\Downloads\PURDUE\SPRING2025\BME450\PROJECT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mattb\Downloads\PURDUE\SPRING2025\BME450\PROJECT\BME450-project\v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B047C80C-CF2C-495E-8693-8E473C12C60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C976926-8C0A-4099-90DE-A76BFE6C772C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,7 +76,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -106,7 +106,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I601"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A481" workbookViewId="0">
-      <selection activeCell="J486" sqref="J486"/>
+    <sheetView tabSelected="1" topLeftCell="A467" workbookViewId="0">
+      <selection activeCell="O482" sqref="O482"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>